<commit_message>
update track marekt price
</commit_message>
<xml_diff>
--- a/data/tracking/코스닥_20250714_history.xlsx
+++ b/data/tracking/코스닥_20250714_history.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -27,6 +27,12 @@
     </font>
     <font>
       <b val="1"/>
+    </font>
+    <font>
+      <color rgb="00FF0000"/>
+    </font>
+    <font>
+      <color rgb="000000FF"/>
     </font>
   </fonts>
   <fills count="2">
@@ -55,11 +61,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C151"/>
+  <dimension ref="A1:E151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +457,16 @@
           <t>2025-07-15</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>2025-07-16</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>2025-07-17</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -464,6 +482,12 @@
       <c r="C2" t="n">
         <v>469000</v>
       </c>
+      <c r="D2" t="n">
+        <v>479000</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>488500</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -479,6 +503,12 @@
       <c r="C3" t="n">
         <v>105000</v>
       </c>
+      <c r="D3" t="n">
+        <v>103100</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>102900</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -494,6 +524,12 @@
       <c r="C4" t="n">
         <v>52100</v>
       </c>
+      <c r="D4" t="n">
+        <v>52000</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>54000</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -509,6 +545,12 @@
       <c r="C5" t="n">
         <v>47200</v>
       </c>
+      <c r="D5" t="n">
+        <v>46450</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>46600</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -524,6 +566,12 @@
       <c r="C6" t="n">
         <v>592000</v>
       </c>
+      <c r="D6" t="n">
+        <v>568000</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>578000</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -539,6 +587,12 @@
       <c r="C7" t="n">
         <v>274000</v>
       </c>
+      <c r="D7" t="n">
+        <v>275500</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>273000</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -554,6 +608,12 @@
       <c r="C8" t="n">
         <v>136600</v>
       </c>
+      <c r="D8" t="n">
+        <v>133800</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>138800</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -569,6 +629,12 @@
       <c r="C9" t="n">
         <v>235000</v>
       </c>
+      <c r="D9" t="n">
+        <v>238500</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>283500</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -584,6 +650,12 @@
       <c r="C10" t="n">
         <v>357500</v>
       </c>
+      <c r="D10" t="n">
+        <v>354000</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>355000</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -599,6 +671,12 @@
       <c r="C11" t="n">
         <v>51600</v>
       </c>
+      <c r="D11" t="n">
+        <v>53400</v>
+      </c>
+      <c r="E11" s="3" t="n">
+        <v>50500</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -614,6 +692,12 @@
       <c r="C12" t="n">
         <v>166000</v>
       </c>
+      <c r="D12" t="n">
+        <v>163600</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>170300</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -629,6 +713,12 @@
       <c r="C13" t="n">
         <v>58900</v>
       </c>
+      <c r="D13" t="n">
+        <v>60200</v>
+      </c>
+      <c r="E13" s="3" t="n">
+        <v>59400</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -644,6 +734,12 @@
       <c r="C14" t="n">
         <v>56100</v>
       </c>
+      <c r="D14" t="n">
+        <v>52700</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>52800</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -659,6 +755,12 @@
       <c r="C15" t="n">
         <v>72100</v>
       </c>
+      <c r="D15" t="n">
+        <v>70100</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>73000</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -674,6 +776,12 @@
       <c r="C16" t="n">
         <v>133700</v>
       </c>
+      <c r="D16" t="n">
+        <v>131200</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>131700</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -689,6 +797,12 @@
       <c r="C17" t="n">
         <v>75800</v>
       </c>
+      <c r="D17" t="n">
+        <v>73900</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>74200</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -704,6 +818,12 @@
       <c r="C18" t="n">
         <v>213000</v>
       </c>
+      <c r="D18" t="n">
+        <v>220500</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>224500</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -719,6 +839,12 @@
       <c r="C19" t="n">
         <v>39450</v>
       </c>
+      <c r="D19" t="n">
+        <v>38600</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>39550</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -734,6 +860,12 @@
       <c r="C20" t="n">
         <v>58500</v>
       </c>
+      <c r="D20" t="n">
+        <v>58500</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>60000</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -749,6 +881,12 @@
       <c r="C21" t="n">
         <v>53700</v>
       </c>
+      <c r="D21" t="n">
+        <v>53000</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>54400</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -764,6 +902,12 @@
       <c r="C22" t="n">
         <v>48200</v>
       </c>
+      <c r="D22" t="n">
+        <v>47275</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>50400</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -779,6 +923,12 @@
       <c r="C23" t="n">
         <v>127100</v>
       </c>
+      <c r="D23" t="n">
+        <v>125000</v>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>127700</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -794,6 +944,12 @@
       <c r="C24" t="n">
         <v>26050</v>
       </c>
+      <c r="D24" t="n">
+        <v>26000</v>
+      </c>
+      <c r="E24" s="3" t="n">
+        <v>25900</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -809,6 +965,12 @@
       <c r="C25" t="n">
         <v>303000</v>
       </c>
+      <c r="D25" t="n">
+        <v>303500</v>
+      </c>
+      <c r="E25" s="3" t="n">
+        <v>295000</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -824,6 +986,12 @@
       <c r="C26" t="n">
         <v>69000</v>
       </c>
+      <c r="D26" t="n">
+        <v>68700</v>
+      </c>
+      <c r="E26" s="3" t="n">
+        <v>68600</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -839,6 +1007,12 @@
       <c r="C27" t="n">
         <v>27250</v>
       </c>
+      <c r="D27" t="n">
+        <v>27050</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>27100</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -854,6 +1028,12 @@
       <c r="C28" t="n">
         <v>85900</v>
       </c>
+      <c r="D28" t="n">
+        <v>87800</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>88900</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -869,6 +1049,12 @@
       <c r="C29" t="n">
         <v>32300</v>
       </c>
+      <c r="D29" t="n">
+        <v>32250</v>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>32550</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -884,6 +1070,12 @@
       <c r="C30" t="n">
         <v>86800</v>
       </c>
+      <c r="D30" t="n">
+        <v>84800</v>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>85100</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -899,6 +1091,12 @@
       <c r="C31" t="n">
         <v>30950</v>
       </c>
+      <c r="D31" t="n">
+        <v>31300</v>
+      </c>
+      <c r="E31" t="n">
+        <v>31300</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -914,6 +1112,12 @@
       <c r="C32" t="n">
         <v>69900</v>
       </c>
+      <c r="D32" t="n">
+        <v>69500</v>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>69700</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -929,6 +1133,12 @@
       <c r="C33" t="n">
         <v>197000</v>
       </c>
+      <c r="D33" t="n">
+        <v>212500</v>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>214000</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -944,6 +1154,12 @@
       <c r="C34" t="n">
         <v>17500</v>
       </c>
+      <c r="D34" t="n">
+        <v>17430</v>
+      </c>
+      <c r="E34" s="3" t="n">
+        <v>17370</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -959,6 +1175,12 @@
       <c r="C35" t="n">
         <v>47400</v>
       </c>
+      <c r="D35" t="n">
+        <v>46650</v>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v>47100</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -974,6 +1196,12 @@
       <c r="C36" t="n">
         <v>30400</v>
       </c>
+      <c r="D36" t="n">
+        <v>30525</v>
+      </c>
+      <c r="E36" s="3" t="n">
+        <v>30350</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -989,6 +1217,12 @@
       <c r="C37" t="n">
         <v>57300</v>
       </c>
+      <c r="D37" t="n">
+        <v>56100</v>
+      </c>
+      <c r="E37" s="3" t="n">
+        <v>55900</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1004,6 +1238,12 @@
       <c r="C38" t="n">
         <v>29150</v>
       </c>
+      <c r="D38" t="n">
+        <v>29750</v>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>30100</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1019,6 +1259,12 @@
       <c r="C39" t="n">
         <v>46750</v>
       </c>
+      <c r="D39" t="n">
+        <v>46300</v>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>47550</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1034,6 +1280,12 @@
       <c r="C40" t="n">
         <v>65700</v>
       </c>
+      <c r="D40" t="n">
+        <v>64700</v>
+      </c>
+      <c r="E40" s="3" t="n">
+        <v>59800</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1049,6 +1301,12 @@
       <c r="C41" t="n">
         <v>36500</v>
       </c>
+      <c r="D41" t="n">
+        <v>36350</v>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>38000</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1064,6 +1322,12 @@
       <c r="C42" t="n">
         <v>22100</v>
       </c>
+      <c r="D42" t="n">
+        <v>21950</v>
+      </c>
+      <c r="E42" s="3" t="n">
+        <v>21000</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1079,6 +1343,12 @@
       <c r="C43" t="n">
         <v>56800</v>
       </c>
+      <c r="D43" t="n">
+        <v>55900</v>
+      </c>
+      <c r="E43" s="3" t="n">
+        <v>55700</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1094,6 +1364,12 @@
       <c r="C44" t="n">
         <v>20750</v>
       </c>
+      <c r="D44" t="n">
+        <v>20150</v>
+      </c>
+      <c r="E44" s="2" t="n">
+        <v>20500</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1109,6 +1385,12 @@
       <c r="C45" t="n">
         <v>43200</v>
       </c>
+      <c r="D45" t="n">
+        <v>42800</v>
+      </c>
+      <c r="E45" s="2" t="n">
+        <v>43900</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1124,6 +1406,12 @@
       <c r="C46" t="n">
         <v>161300</v>
       </c>
+      <c r="D46" t="n">
+        <v>163000</v>
+      </c>
+      <c r="E46" s="3" t="n">
+        <v>162200</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1139,6 +1427,12 @@
       <c r="C47" t="n">
         <v>32300</v>
       </c>
+      <c r="D47" t="n">
+        <v>32400</v>
+      </c>
+      <c r="E47" s="2" t="n">
+        <v>34650</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1154,6 +1448,12 @@
       <c r="C48" t="n">
         <v>10350</v>
       </c>
+      <c r="D48" t="n">
+        <v>10210</v>
+      </c>
+      <c r="E48" s="2" t="n">
+        <v>10320</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1169,6 +1469,12 @@
       <c r="C49" t="n">
         <v>100100</v>
       </c>
+      <c r="D49" t="n">
+        <v>100600</v>
+      </c>
+      <c r="E49" s="3" t="n">
+        <v>99200</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1184,6 +1490,12 @@
       <c r="C50" t="n">
         <v>33350</v>
       </c>
+      <c r="D50" t="n">
+        <v>33700</v>
+      </c>
+      <c r="E50" s="3" t="n">
+        <v>33550</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1199,6 +1511,12 @@
       <c r="C51" t="n">
         <v>70700</v>
       </c>
+      <c r="D51" t="n">
+        <v>70000</v>
+      </c>
+      <c r="E51" t="n">
+        <v>70000</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1214,6 +1532,12 @@
       <c r="C52" t="n">
         <v>37050</v>
       </c>
+      <c r="D52" t="n">
+        <v>37950</v>
+      </c>
+      <c r="E52" s="2" t="n">
+        <v>40900</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1229,6 +1553,12 @@
       <c r="C53" t="n">
         <v>45500</v>
       </c>
+      <c r="D53" t="n">
+        <v>45050</v>
+      </c>
+      <c r="E53" s="2" t="n">
+        <v>45100</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1244,6 +1574,12 @@
       <c r="C54" t="n">
         <v>30000</v>
       </c>
+      <c r="D54" t="n">
+        <v>29650</v>
+      </c>
+      <c r="E54" s="3" t="n">
+        <v>29300</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1259,6 +1595,12 @@
       <c r="C55" t="n">
         <v>12570</v>
       </c>
+      <c r="D55" t="n">
+        <v>12650</v>
+      </c>
+      <c r="E55" s="2" t="n">
+        <v>12660</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1274,6 +1616,12 @@
       <c r="C56" t="n">
         <v>35800</v>
       </c>
+      <c r="D56" t="n">
+        <v>36950</v>
+      </c>
+      <c r="E56" s="3" t="n">
+        <v>35700</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1289,6 +1637,12 @@
       <c r="C57" t="n">
         <v>95400</v>
       </c>
+      <c r="D57" t="n">
+        <v>93400</v>
+      </c>
+      <c r="E57" s="3" t="n">
+        <v>93200</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1304,6 +1658,12 @@
       <c r="C58" t="n">
         <v>10830</v>
       </c>
+      <c r="D58" t="n">
+        <v>10590</v>
+      </c>
+      <c r="E58" s="3" t="n">
+        <v>10390</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1319,6 +1679,12 @@
       <c r="C59" t="n">
         <v>17710</v>
       </c>
+      <c r="D59" t="n">
+        <v>17580</v>
+      </c>
+      <c r="E59" s="3" t="n">
+        <v>17240</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1334,6 +1700,12 @@
       <c r="C60" t="n">
         <v>14840</v>
       </c>
+      <c r="D60" t="n">
+        <v>14980</v>
+      </c>
+      <c r="E60" s="2" t="n">
+        <v>15260</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1349,6 +1721,12 @@
       <c r="C61" t="n">
         <v>49450</v>
       </c>
+      <c r="D61" t="n">
+        <v>48850</v>
+      </c>
+      <c r="E61" s="2" t="n">
+        <v>49250</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1364,6 +1742,12 @@
       <c r="C62" t="n">
         <v>14360</v>
       </c>
+      <c r="D62" t="n">
+        <v>14240</v>
+      </c>
+      <c r="E62" s="3" t="n">
+        <v>14220</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1379,6 +1763,12 @@
       <c r="C63" t="n">
         <v>42800</v>
       </c>
+      <c r="D63" t="n">
+        <v>45900</v>
+      </c>
+      <c r="E63" s="2" t="n">
+        <v>46150</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1394,6 +1784,12 @@
       <c r="C64" t="n">
         <v>12220</v>
       </c>
+      <c r="D64" t="n">
+        <v>12160</v>
+      </c>
+      <c r="E64" s="2" t="n">
+        <v>12230</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1409,6 +1805,12 @@
       <c r="C65" t="n">
         <v>24850</v>
       </c>
+      <c r="D65" t="n">
+        <v>24750</v>
+      </c>
+      <c r="E65" s="2" t="n">
+        <v>24800</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1424,6 +1826,12 @@
       <c r="C66" t="n">
         <v>9540</v>
       </c>
+      <c r="D66" t="n">
+        <v>9345</v>
+      </c>
+      <c r="E66" s="3" t="n">
+        <v>9270</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1439,6 +1847,12 @@
       <c r="C67" t="n">
         <v>37200</v>
       </c>
+      <c r="D67" t="n">
+        <v>41450</v>
+      </c>
+      <c r="E67" s="3" t="n">
+        <v>40850</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1454,6 +1868,12 @@
       <c r="C68" t="n">
         <v>39200</v>
       </c>
+      <c r="D68" t="n">
+        <v>45650</v>
+      </c>
+      <c r="E68" s="3" t="n">
+        <v>43250</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1469,6 +1889,12 @@
       <c r="C69" t="n">
         <v>18410</v>
       </c>
+      <c r="D69" t="n">
+        <v>18170</v>
+      </c>
+      <c r="E69" s="2" t="n">
+        <v>18660</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1484,6 +1910,12 @@
       <c r="C70" t="n">
         <v>28950</v>
       </c>
+      <c r="D70" t="n">
+        <v>27450</v>
+      </c>
+      <c r="E70" s="2" t="n">
+        <v>27600</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1499,6 +1931,12 @@
       <c r="C71" t="n">
         <v>10200</v>
       </c>
+      <c r="D71" t="n">
+        <v>10280</v>
+      </c>
+      <c r="E71" s="2" t="n">
+        <v>11690</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -1514,6 +1952,12 @@
       <c r="C72" t="n">
         <v>35100</v>
       </c>
+      <c r="D72" t="n">
+        <v>34750</v>
+      </c>
+      <c r="E72" s="3" t="n">
+        <v>34150</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1529,6 +1973,12 @@
       <c r="C73" t="n">
         <v>32350</v>
       </c>
+      <c r="D73" t="n">
+        <v>31850</v>
+      </c>
+      <c r="E73" s="3" t="n">
+        <v>31800</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -1544,6 +1994,12 @@
       <c r="C74" t="n">
         <v>11750</v>
       </c>
+      <c r="D74" t="n">
+        <v>11760</v>
+      </c>
+      <c r="E74" s="2" t="n">
+        <v>11770</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -1559,6 +2015,12 @@
       <c r="C75" t="n">
         <v>28400</v>
       </c>
+      <c r="D75" t="n">
+        <v>29050</v>
+      </c>
+      <c r="E75" s="2" t="n">
+        <v>29700</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -1574,6 +2036,12 @@
       <c r="C76" t="n">
         <v>31200</v>
       </c>
+      <c r="D76" t="n">
+        <v>31100</v>
+      </c>
+      <c r="E76" s="2" t="n">
+        <v>32300</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -1589,6 +2057,12 @@
       <c r="C77" t="n">
         <v>36100</v>
       </c>
+      <c r="D77" t="n">
+        <v>35500</v>
+      </c>
+      <c r="E77" s="3" t="n">
+        <v>35200</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -1604,6 +2078,12 @@
       <c r="C78" t="n">
         <v>69200</v>
       </c>
+      <c r="D78" t="n">
+        <v>66700</v>
+      </c>
+      <c r="E78" s="2" t="n">
+        <v>68400</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -1619,6 +2099,12 @@
       <c r="C79" t="n">
         <v>66700</v>
       </c>
+      <c r="D79" t="n">
+        <v>66500</v>
+      </c>
+      <c r="E79" s="2" t="n">
+        <v>67000</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -1634,6 +2120,12 @@
       <c r="C80" t="n">
         <v>11090</v>
       </c>
+      <c r="D80" t="n">
+        <v>11200</v>
+      </c>
+      <c r="E80" s="3" t="n">
+        <v>11080</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -1649,6 +2141,12 @@
       <c r="C81" t="n">
         <v>18440</v>
       </c>
+      <c r="D81" t="n">
+        <v>17890</v>
+      </c>
+      <c r="E81" s="3" t="n">
+        <v>17670</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -1664,6 +2162,12 @@
       <c r="C82" t="n">
         <v>10690</v>
       </c>
+      <c r="D82" t="n">
+        <v>10530</v>
+      </c>
+      <c r="E82" s="3" t="n">
+        <v>10490</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -1679,6 +2183,12 @@
       <c r="C83" t="n">
         <v>27550</v>
       </c>
+      <c r="D83" t="n">
+        <v>28650</v>
+      </c>
+      <c r="E83" t="n">
+        <v>28650</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -1694,6 +2204,12 @@
       <c r="C84" t="n">
         <v>25500</v>
       </c>
+      <c r="D84" t="n">
+        <v>25750</v>
+      </c>
+      <c r="E84" s="3" t="n">
+        <v>25000</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -1709,6 +2225,12 @@
       <c r="C85" t="n">
         <v>29050</v>
       </c>
+      <c r="D85" t="n">
+        <v>28900</v>
+      </c>
+      <c r="E85" s="3" t="n">
+        <v>28300</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -1724,6 +2246,12 @@
       <c r="C86" t="n">
         <v>15470</v>
       </c>
+      <c r="D86" t="n">
+        <v>15770</v>
+      </c>
+      <c r="E86" s="2" t="n">
+        <v>16200</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -1739,6 +2267,12 @@
       <c r="C87" t="n">
         <v>66000</v>
       </c>
+      <c r="D87" t="n">
+        <v>68900</v>
+      </c>
+      <c r="E87" s="3" t="n">
+        <v>67000</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -1754,6 +2288,12 @@
       <c r="C88" t="n">
         <v>13700</v>
       </c>
+      <c r="D88" t="n">
+        <v>13960</v>
+      </c>
+      <c r="E88" s="2" t="n">
+        <v>14020</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -1769,6 +2309,12 @@
       <c r="C89" t="n">
         <v>7930</v>
       </c>
+      <c r="D89" t="n">
+        <v>8050</v>
+      </c>
+      <c r="E89" s="2" t="n">
+        <v>8070</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -1784,6 +2330,12 @@
       <c r="C90" t="n">
         <v>22550</v>
       </c>
+      <c r="D90" t="n">
+        <v>22650</v>
+      </c>
+      <c r="E90" s="2" t="n">
+        <v>22900</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -1799,6 +2351,12 @@
       <c r="C91" t="n">
         <v>9750</v>
       </c>
+      <c r="D91" t="n">
+        <v>9610</v>
+      </c>
+      <c r="E91" s="2" t="n">
+        <v>9870</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -1814,6 +2372,12 @@
       <c r="C92" t="n">
         <v>7400</v>
       </c>
+      <c r="D92" t="n">
+        <v>7300</v>
+      </c>
+      <c r="E92" s="3" t="n">
+        <v>7230</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -1829,6 +2393,12 @@
       <c r="C93" t="n">
         <v>49450</v>
       </c>
+      <c r="D93" t="n">
+        <v>50100</v>
+      </c>
+      <c r="E93" t="n">
+        <v>50100</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -1844,6 +2414,12 @@
       <c r="C94" t="n">
         <v>39750</v>
       </c>
+      <c r="D94" t="n">
+        <v>40200</v>
+      </c>
+      <c r="E94" s="3" t="n">
+        <v>39550</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -1859,6 +2435,12 @@
       <c r="C95" t="n">
         <v>49600</v>
       </c>
+      <c r="D95" t="n">
+        <v>48950</v>
+      </c>
+      <c r="E95" s="2" t="n">
+        <v>49300</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -1874,6 +2456,12 @@
       <c r="C96" t="n">
         <v>26800</v>
       </c>
+      <c r="D96" t="n">
+        <v>26950</v>
+      </c>
+      <c r="E96" s="3" t="n">
+        <v>26600</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -1889,6 +2477,12 @@
       <c r="C97" t="n">
         <v>50600</v>
       </c>
+      <c r="D97" t="n">
+        <v>51200</v>
+      </c>
+      <c r="E97" s="3" t="n">
+        <v>51000</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -1904,6 +2498,12 @@
       <c r="C98" t="n">
         <v>7410</v>
       </c>
+      <c r="D98" t="n">
+        <v>7390</v>
+      </c>
+      <c r="E98" s="2" t="n">
+        <v>7400</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -1919,6 +2519,12 @@
       <c r="C99" t="n">
         <v>20450</v>
       </c>
+      <c r="D99" t="n">
+        <v>20300</v>
+      </c>
+      <c r="E99" s="2" t="n">
+        <v>20850</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -1934,6 +2540,12 @@
       <c r="C100" t="n">
         <v>24100</v>
       </c>
+      <c r="D100" t="n">
+        <v>24600</v>
+      </c>
+      <c r="E100" s="2" t="n">
+        <v>24700</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -1949,6 +2561,12 @@
       <c r="C101" t="n">
         <v>25550</v>
       </c>
+      <c r="D101" t="n">
+        <v>25150</v>
+      </c>
+      <c r="E101" s="2" t="n">
+        <v>25300</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -1964,6 +2582,12 @@
       <c r="C102" t="n">
         <v>13630</v>
       </c>
+      <c r="D102" t="n">
+        <v>14270</v>
+      </c>
+      <c r="E102" s="2" t="n">
+        <v>14860</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -1979,6 +2603,12 @@
       <c r="C103" t="n">
         <v>16100</v>
       </c>
+      <c r="D103" t="n">
+        <v>16155</v>
+      </c>
+      <c r="E103" s="2" t="n">
+        <v>16280</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -1994,6 +2624,12 @@
       <c r="C104" t="n">
         <v>14930</v>
       </c>
+      <c r="D104" t="n">
+        <v>15060</v>
+      </c>
+      <c r="E104" s="2" t="n">
+        <v>15080</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -2009,6 +2645,12 @@
       <c r="C105" t="n">
         <v>40750</v>
       </c>
+      <c r="D105" t="n">
+        <v>40850</v>
+      </c>
+      <c r="E105" t="n">
+        <v>40850</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -2024,6 +2666,12 @@
       <c r="C106" t="n">
         <v>26600</v>
       </c>
+      <c r="D106" t="n">
+        <v>27950</v>
+      </c>
+      <c r="E106" s="3" t="n">
+        <v>26950</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -2039,6 +2687,12 @@
       <c r="C107" t="n">
         <v>20300</v>
       </c>
+      <c r="D107" t="n">
+        <v>19940</v>
+      </c>
+      <c r="E107" s="3" t="n">
+        <v>19470</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -2054,6 +2708,12 @@
       <c r="C108" t="n">
         <v>44500</v>
       </c>
+      <c r="D108" t="n">
+        <v>44000</v>
+      </c>
+      <c r="E108" s="3" t="n">
+        <v>43450</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -2069,6 +2729,12 @@
       <c r="C109" t="n">
         <v>16500</v>
       </c>
+      <c r="D109" t="n">
+        <v>16320</v>
+      </c>
+      <c r="E109" s="2" t="n">
+        <v>17680</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -2084,6 +2750,12 @@
       <c r="C110" t="n">
         <v>3210</v>
       </c>
+      <c r="D110" t="n">
+        <v>3200</v>
+      </c>
+      <c r="E110" s="2" t="n">
+        <v>3225</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -2099,6 +2771,12 @@
       <c r="C111" t="n">
         <v>6170</v>
       </c>
+      <c r="D111" t="n">
+        <v>6070</v>
+      </c>
+      <c r="E111" s="2" t="n">
+        <v>6140</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -2114,6 +2792,12 @@
       <c r="C112" t="n">
         <v>45800</v>
       </c>
+      <c r="D112" t="n">
+        <v>45600</v>
+      </c>
+      <c r="E112" s="2" t="n">
+        <v>46050</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -2129,6 +2813,12 @@
       <c r="C113" t="n">
         <v>49100</v>
       </c>
+      <c r="D113" t="n">
+        <v>48650</v>
+      </c>
+      <c r="E113" s="3" t="n">
+        <v>48600</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -2144,6 +2834,12 @@
       <c r="C114" t="n">
         <v>51200</v>
       </c>
+      <c r="D114" t="n">
+        <v>51700</v>
+      </c>
+      <c r="E114" s="2" t="n">
+        <v>52000</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -2159,6 +2855,12 @@
       <c r="C115" t="n">
         <v>27300</v>
       </c>
+      <c r="D115" t="n">
+        <v>27700</v>
+      </c>
+      <c r="E115" s="2" t="n">
+        <v>30300</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -2174,6 +2876,12 @@
       <c r="C116" t="n">
         <v>11810</v>
       </c>
+      <c r="D116" t="n">
+        <v>11590</v>
+      </c>
+      <c r="E116" s="2" t="n">
+        <v>11640</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -2189,6 +2897,12 @@
       <c r="C117" t="n">
         <v>18720</v>
       </c>
+      <c r="D117" t="n">
+        <v>18690</v>
+      </c>
+      <c r="E117" s="2" t="n">
+        <v>18700</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -2204,6 +2918,12 @@
       <c r="C118" t="n">
         <v>25450</v>
       </c>
+      <c r="D118" t="n">
+        <v>25450</v>
+      </c>
+      <c r="E118" t="n">
+        <v>25450</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -2219,6 +2939,12 @@
       <c r="C119" t="n">
         <v>24300</v>
       </c>
+      <c r="D119" t="n">
+        <v>25150</v>
+      </c>
+      <c r="E119" s="3" t="n">
+        <v>25100</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -2234,6 +2960,12 @@
       <c r="C120" t="n">
         <v>75200</v>
       </c>
+      <c r="D120" t="n">
+        <v>74800</v>
+      </c>
+      <c r="E120" s="3" t="n">
+        <v>74200</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -2249,6 +2981,12 @@
       <c r="C121" t="n">
         <v>100100</v>
       </c>
+      <c r="D121" t="n">
+        <v>100300</v>
+      </c>
+      <c r="E121" s="2" t="n">
+        <v>101400</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -2264,6 +3002,12 @@
       <c r="C122" t="n">
         <v>46050</v>
       </c>
+      <c r="D122" t="n">
+        <v>44700</v>
+      </c>
+      <c r="E122" s="2" t="n">
+        <v>47250</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -2279,6 +3023,12 @@
       <c r="C123" t="n">
         <v>15190</v>
       </c>
+      <c r="D123" t="n">
+        <v>15100</v>
+      </c>
+      <c r="E123" s="2" t="n">
+        <v>15180</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -2294,6 +3044,12 @@
       <c r="C124" t="n">
         <v>25450</v>
       </c>
+      <c r="D124" t="n">
+        <v>26600</v>
+      </c>
+      <c r="E124" s="3" t="n">
+        <v>25550</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -2309,6 +3065,12 @@
       <c r="C125" t="n">
         <v>8690</v>
       </c>
+      <c r="D125" t="n">
+        <v>8590</v>
+      </c>
+      <c r="E125" s="3" t="n">
+        <v>8510</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -2324,6 +3086,12 @@
       <c r="C126" t="n">
         <v>21850</v>
       </c>
+      <c r="D126" t="n">
+        <v>22450</v>
+      </c>
+      <c r="E126" s="3" t="n">
+        <v>22200</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -2339,6 +3107,12 @@
       <c r="C127" t="n">
         <v>6900</v>
       </c>
+      <c r="D127" t="n">
+        <v>6840</v>
+      </c>
+      <c r="E127" s="2" t="n">
+        <v>6980</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -2354,6 +3128,12 @@
       <c r="C128" t="n">
         <v>39200</v>
       </c>
+      <c r="D128" t="n">
+        <v>39350</v>
+      </c>
+      <c r="E128" s="2" t="n">
+        <v>39500</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -2369,6 +3149,12 @@
       <c r="C129" t="n">
         <v>35250</v>
       </c>
+      <c r="D129" t="n">
+        <v>37200</v>
+      </c>
+      <c r="E129" s="3" t="n">
+        <v>37050</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -2384,6 +3170,12 @@
       <c r="C130" t="n">
         <v>7350</v>
       </c>
+      <c r="D130" t="n">
+        <v>7180</v>
+      </c>
+      <c r="E130" s="2" t="n">
+        <v>7190</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -2399,6 +3191,12 @@
       <c r="C131" t="n">
         <v>12690</v>
       </c>
+      <c r="D131" t="n">
+        <v>12690</v>
+      </c>
+      <c r="E131" s="2" t="n">
+        <v>12770</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -2414,6 +3212,12 @@
       <c r="C132" t="n">
         <v>40100</v>
       </c>
+      <c r="D132" t="n">
+        <v>40100</v>
+      </c>
+      <c r="E132" s="2" t="n">
+        <v>40200</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -2429,6 +3233,12 @@
       <c r="C133" t="n">
         <v>21200</v>
       </c>
+      <c r="D133" t="n">
+        <v>20950</v>
+      </c>
+      <c r="E133" s="2" t="n">
+        <v>21050</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -2444,6 +3254,12 @@
       <c r="C134" t="n">
         <v>14300</v>
       </c>
+      <c r="D134" t="n">
+        <v>14240</v>
+      </c>
+      <c r="E134" s="3" t="n">
+        <v>14160</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -2459,6 +3275,12 @@
       <c r="C135" t="n">
         <v>8840</v>
       </c>
+      <c r="D135" t="n">
+        <v>8870</v>
+      </c>
+      <c r="E135" s="2" t="n">
+        <v>9100</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -2474,6 +3296,12 @@
       <c r="C136" t="n">
         <v>6530</v>
       </c>
+      <c r="D136" t="n">
+        <v>6520</v>
+      </c>
+      <c r="E136" s="2" t="n">
+        <v>6560</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -2489,6 +3317,12 @@
       <c r="C137" t="n">
         <v>14670</v>
       </c>
+      <c r="D137" t="n">
+        <v>14470</v>
+      </c>
+      <c r="E137" s="2" t="n">
+        <v>15200</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -2504,6 +3338,12 @@
       <c r="C138" t="n">
         <v>18920</v>
       </c>
+      <c r="D138" t="n">
+        <v>18770</v>
+      </c>
+      <c r="E138" s="3" t="n">
+        <v>17970</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -2519,6 +3359,12 @@
       <c r="C139" t="n">
         <v>38350</v>
       </c>
+      <c r="D139" t="n">
+        <v>39350</v>
+      </c>
+      <c r="E139" s="3" t="n">
+        <v>39300</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -2534,6 +3380,12 @@
       <c r="C140" t="n">
         <v>8880</v>
       </c>
+      <c r="D140" t="n">
+        <v>8810</v>
+      </c>
+      <c r="E140" s="2" t="n">
+        <v>9010</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -2549,6 +3401,12 @@
       <c r="C141" t="n">
         <v>4075</v>
       </c>
+      <c r="D141" t="n">
+        <v>4105</v>
+      </c>
+      <c r="E141" t="n">
+        <v>4105</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -2564,6 +3422,12 @@
       <c r="C142" t="n">
         <v>15660</v>
       </c>
+      <c r="D142" t="n">
+        <v>15390</v>
+      </c>
+      <c r="E142" t="n">
+        <v>15390</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -2579,6 +3443,12 @@
       <c r="C143" t="n">
         <v>38750</v>
       </c>
+      <c r="D143" t="n">
+        <v>38700</v>
+      </c>
+      <c r="E143" s="2" t="n">
+        <v>38750</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -2594,6 +3464,12 @@
       <c r="C144" t="n">
         <v>24850</v>
       </c>
+      <c r="D144" t="n">
+        <v>25150</v>
+      </c>
+      <c r="E144" s="2" t="n">
+        <v>25250</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -2609,6 +3485,12 @@
       <c r="C145" t="n">
         <v>17570</v>
       </c>
+      <c r="D145" t="n">
+        <v>17180</v>
+      </c>
+      <c r="E145" s="2" t="n">
+        <v>17220</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -2624,6 +3506,12 @@
       <c r="C146" t="n">
         <v>12550</v>
       </c>
+      <c r="D146" t="n">
+        <v>12590</v>
+      </c>
+      <c r="E146" s="2" t="n">
+        <v>13190</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -2639,6 +3527,12 @@
       <c r="C147" t="n">
         <v>26000</v>
       </c>
+      <c r="D147" t="n">
+        <v>27950</v>
+      </c>
+      <c r="E147" s="2" t="n">
+        <v>28500</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -2654,6 +3548,12 @@
       <c r="C148" t="n">
         <v>17090</v>
       </c>
+      <c r="D148" t="n">
+        <v>17000</v>
+      </c>
+      <c r="E148" s="3" t="n">
+        <v>16950</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -2669,6 +3569,12 @@
       <c r="C149" t="n">
         <v>13270</v>
       </c>
+      <c r="D149" t="n">
+        <v>13460</v>
+      </c>
+      <c r="E149" s="3" t="n">
+        <v>13400</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -2684,6 +3590,12 @@
       <c r="C150" t="n">
         <v>8200</v>
       </c>
+      <c r="D150" t="n">
+        <v>8130</v>
+      </c>
+      <c r="E150" t="n">
+        <v>8130</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -2698,6 +3610,12 @@
       </c>
       <c r="C151" t="n">
         <v>10730</v>
+      </c>
+      <c r="D151" t="n">
+        <v>10550</v>
+      </c>
+      <c r="E151" s="2" t="n">
+        <v>10570</v>
       </c>
     </row>
   </sheetData>

</xml_diff>